<commit_message>
added screenshot in extent reports
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\FlipkartAutomation\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\Shopping\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEE43EA-F821-4498-BE30-439B23BCE12C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966A40E2-03D0-456F-9045-835667F38F58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -90,7 +90,13 @@
     <t>9966671896</t>
   </si>
   <si>
-    <t>jR@1372jitu</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t>hhfgfgf</t>
+  </si>
+  <si>
+    <t>kjjkhjghfgf</t>
   </si>
 </sst>
 </file>
@@ -531,7 +537,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +572,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -651,7 +657,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +675,7 @@
         <v>9732097320</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -698,7 +704,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +734,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
@@ -742,16 +748,16 @@
         <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId1" display="jR@1372jitu" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" display="jR@1372jitu" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>